<commit_message>
add prep_wastewater_data to clean
</commit_message>
<xml_diff>
--- a/flow/data/WW_Discharge_Key.xlsx
+++ b/flow/data/WW_Discharge_Key.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mong275\Local Files\Sankey_Notebook_Development\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mong275\Local Files\Repos\flow\flow\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3BCD8D-FD1A-40CA-9F40-72064D168569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A295A88-8AD9-4AB5-928C-7B158B8E1EF8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-495" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{32AD0BB4-0F32-41B3-AC5F-F2F8BB635B4F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>DISCHARGE_METHOD</t>
   </si>
@@ -107,24 +107,15 @@
     <t>Industrial</t>
   </si>
   <si>
-    <t>Consumption</t>
-  </si>
-  <si>
     <t>Agriculture</t>
   </si>
   <si>
-    <t>WW</t>
-  </si>
-  <si>
     <t>Public Water Supply</t>
   </si>
   <si>
     <t>Discharge To Another Facility</t>
   </si>
   <si>
-    <t>TEC</t>
-  </si>
-  <si>
     <t>Discharge To Groundwater</t>
   </si>
   <si>
@@ -138,13 +129,63 @@
   </si>
   <si>
     <t>No Discharge</t>
+  </si>
+  <si>
+    <t>Irrigation</t>
+  </si>
+  <si>
+    <t>Wastewater</t>
+  </si>
+  <si>
+    <r>
+      <t>Indirect potable reuse: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF202124"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>Uses an environmental buffer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF202124"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>, such as a lake, river, or a groundwater aquifer, before the water is treated at a drinking water treatment plant. Direct potable reuse: Involves the treatment and distribution of water without an environmental buffer.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Non-potable water reuse – Water is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF202124"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>captured, treated, and used for non-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF202124"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>drinking purposes, such as toilet flushing, clothes washing, and irrigation.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +200,28 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF202124"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF202124"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF202124"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF202124"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -196,12 +259,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,19 +581,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC2B6AD-D417-4C2C-AC7C-895F37397C29}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="37.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,7 +601,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -544,7 +609,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -552,7 +617,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -560,7 +625,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -568,31 +633,31 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -600,15 +665,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -616,7 +681,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -624,7 +689,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -632,47 +697,53 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -680,44 +751,44 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>